<commit_message>
Scaled ARpUIiRC based on VA's share of national coal capacity
</commit_message>
<xml_diff>
--- a/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
+++ b/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ARpUIiRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\elec\ARpUIiRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="9030" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="316">
   <si>
     <t>ARpUIiRC Annual Retirement per Unit Increase in Relative Cost</t>
   </si>
@@ -980,6 +980,18 @@
   </si>
   <si>
     <t>results in the EPS requires a value of 4000 MW/($/MWh) for coal units)</t>
+  </si>
+  <si>
+    <t>State Adjustment</t>
+  </si>
+  <si>
+    <t>Weighting factor</t>
+  </si>
+  <si>
+    <t>State coal capacity, start year</t>
+  </si>
+  <si>
+    <t>US coal capacity, start year (see US EPS 3.0, elec/SYC)</t>
   </si>
 </sst>
 </file>
@@ -1561,18 +1573,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1585,30 +1597,30 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="30" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="29" t="s">
         <v>278</v>
       </c>
@@ -1618,192 +1630,192 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" s="30" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>0.9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>259</v>
       </c>
@@ -1829,14 +1841,14 @@
       <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="13" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" style="13" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="42.73046875" style="13" customWidth="1"/>
     <col min="3" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="14" t="s">
         <v>252</v>
       </c>
@@ -1937,14 +1949,14 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="16" t="s">
         <v>122</v>
       </c>
@@ -1955,7 +1967,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>124</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="16" t="s">
         <v>125</v>
       </c>
@@ -1979,7 +1991,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="16" t="s">
         <v>127</v>
       </c>
@@ -1990,7 +2002,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="17" t="s">
         <v>129</v>
       </c>
@@ -1998,12 +2010,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="14" t="s">
         <v>132</v>
       </c>
@@ -2107,7 +2119,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="15" t="s">
         <v>134</v>
       </c>
@@ -2211,18 +2223,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>137</v>
       </c>
@@ -2329,7 +2341,7 @@
         <v>-2.0031E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>139</v>
       </c>
@@ -2436,7 +2448,7 @@
         <v>-1.3575E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
         <v>141</v>
       </c>
@@ -2543,7 +2555,7 @@
         <v>1.6708000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>143</v>
       </c>
@@ -2650,7 +2662,7 @@
         <v>2.7220999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="17" t="s">
         <v>145</v>
       </c>
@@ -2757,7 +2769,7 @@
         <v>-7.1539999999999998E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="17" t="s">
         <v>147</v>
       </c>
@@ -2864,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="17" t="s">
         <v>149</v>
       </c>
@@ -2971,7 +2983,7 @@
         <v>8.5441000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="17" t="s">
         <v>151</v>
       </c>
@@ -3078,7 +3090,7 @@
         <v>1.1962E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="17" t="s">
         <v>153</v>
       </c>
@@ -3185,7 +3197,7 @@
         <v>3.1888E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>155</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>158</v>
       </c>
@@ -3399,12 +3411,12 @@
         <v>1.5689000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
         <v>161</v>
       </c>
@@ -3511,7 +3523,7 @@
         <v>-9.4450000000000003E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
         <v>163</v>
       </c>
@@ -3618,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="17" t="s">
         <v>165</v>
       </c>
@@ -3725,7 +3737,7 @@
         <v>-2.5900000000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="17" t="s">
         <v>166</v>
       </c>
@@ -3832,7 +3844,7 @@
         <v>-4.9399999999999997E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="17" t="s">
         <v>167</v>
       </c>
@@ -3939,7 +3951,7 @@
         <v>-1.6899999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>168</v>
       </c>
@@ -4046,12 +4058,12 @@
         <v>-1.0089999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="17" t="s">
         <v>170</v>
       </c>
@@ -4158,7 +4170,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="17" t="s">
         <v>171</v>
       </c>
@@ -4265,7 +4277,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="17" t="s">
         <v>172</v>
       </c>
@@ -4372,7 +4384,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="17" t="s">
         <v>173</v>
       </c>
@@ -4479,7 +4491,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="17" t="s">
         <v>174</v>
       </c>
@@ -4586,7 +4598,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
         <v>176</v>
       </c>
@@ -4693,7 +4705,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="17" t="s">
         <v>177</v>
       </c>
@@ -4800,7 +4812,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="17" t="s">
         <v>178</v>
       </c>
@@ -4907,7 +4919,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="17" t="s">
         <v>179</v>
       </c>
@@ -5014,7 +5026,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="17" t="s">
         <v>180</v>
       </c>
@@ -5121,7 +5133,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>182</v>
       </c>
@@ -5228,12 +5240,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="17" t="s">
         <v>184</v>
       </c>
@@ -5340,7 +5352,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="17" t="s">
         <v>185</v>
       </c>
@@ -5447,7 +5459,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="17" t="s">
         <v>186</v>
       </c>
@@ -5554,7 +5566,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="17" t="s">
         <v>187</v>
       </c>
@@ -5661,7 +5673,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="17" t="s">
         <v>188</v>
       </c>
@@ -5768,7 +5780,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="17" t="s">
         <v>189</v>
       </c>
@@ -5875,7 +5887,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="17" t="s">
         <v>190</v>
       </c>
@@ -5982,7 +5994,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="17" t="s">
         <v>191</v>
       </c>
@@ -6089,7 +6101,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="17" t="s">
         <v>192</v>
       </c>
@@ -6196,7 +6208,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="17" t="s">
         <v>193</v>
       </c>
@@ -6303,7 +6315,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>194</v>
       </c>
@@ -6410,7 +6422,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>195</v>
       </c>
@@ -6517,12 +6529,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="20" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="17" t="s">
         <v>198</v>
       </c>
@@ -6629,7 +6641,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="17" t="s">
         <v>199</v>
       </c>
@@ -6736,7 +6748,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="17" t="s">
         <v>200</v>
       </c>
@@ -6843,7 +6855,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="17" t="s">
         <v>201</v>
       </c>
@@ -6950,7 +6962,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="17" t="s">
         <v>202</v>
       </c>
@@ -7057,7 +7069,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="17" t="s">
         <v>203</v>
       </c>
@@ -7164,7 +7176,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="17" t="s">
         <v>204</v>
       </c>
@@ -7271,7 +7283,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="17" t="s">
         <v>205</v>
       </c>
@@ -7378,7 +7390,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="17" t="s">
         <v>206</v>
       </c>
@@ -7485,7 +7497,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
         <v>207</v>
       </c>
@@ -7592,7 +7604,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
         <v>208</v>
       </c>
@@ -7699,12 +7711,12 @@
         <v>1.5321E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="20" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="17" t="s">
         <v>211</v>
       </c>
@@ -7811,7 +7823,7 @@
         <v>-1.0508E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="17" t="s">
         <v>212</v>
       </c>
@@ -7918,7 +7930,7 @@
         <v>-2.98E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="17" t="s">
         <v>214</v>
       </c>
@@ -8025,7 +8037,7 @@
         <v>2.3052E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="17" t="s">
         <v>216</v>
       </c>
@@ -8132,7 +8144,7 @@
         <v>-4.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="17" t="s">
         <v>218</v>
       </c>
@@ -8239,7 +8251,7 @@
         <v>4.6114000000000002E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="17" t="s">
         <v>219</v>
       </c>
@@ -8346,7 +8358,7 @@
         <v>4.542E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>221</v>
       </c>
@@ -8453,7 +8465,7 @@
         <v>3.7383E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
         <v>222</v>
       </c>
@@ -8560,8 +8572,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="43" t="s">
         <v>224</v>
       </c>
@@ -8599,122 +8611,122 @@
       <c r="AH87" s="43"/>
       <c r="AI87" s="43"/>
     </row>
-    <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="26" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" s="26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="26" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="26" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B93" s="26" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="26" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="95" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="26" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="26" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="26" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B100" s="26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="26" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B102" s="26" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="26" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="26" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="26" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="26" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="26" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="26" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="26" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="26" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="26" t="s">
         <v>257</v>
       </c>
@@ -8739,14 +8751,14 @@
       <selection pane="bottomRight" activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="13" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" style="13" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="42.73046875" style="13" customWidth="1"/>
     <col min="3" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="14" t="s">
         <v>248</v>
       </c>
@@ -8847,8 +8859,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="16" t="s">
         <v>122</v>
       </c>
@@ -8859,7 +8871,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>124</v>
       </c>
@@ -8872,7 +8884,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="16" t="s">
         <v>125</v>
       </c>
@@ -8883,7 +8895,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="16" t="s">
         <v>127</v>
       </c>
@@ -8894,7 +8906,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="17" t="s">
         <v>129</v>
       </c>
@@ -8902,12 +8914,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="14" t="s">
         <v>132</v>
       </c>
@@ -9011,7 +9023,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="15" t="s">
         <v>134</v>
       </c>
@@ -9115,18 +9127,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>137</v>
       </c>
@@ -9233,7 +9245,7 @@
         <v>-9.3896999999999994E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>139</v>
       </c>
@@ -9340,7 +9352,7 @@
         <v>-2.0216000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
         <v>141</v>
       </c>
@@ -9447,7 +9459,7 @@
         <v>1.6057999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>143</v>
       </c>
@@ -9554,7 +9566,7 @@
         <v>2.4892000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="17" t="s">
         <v>145</v>
       </c>
@@ -9661,7 +9673,7 @@
         <v>-1.3489999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="17" t="s">
         <v>147</v>
       </c>
@@ -9768,7 +9780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="17" t="s">
         <v>149</v>
       </c>
@@ -9875,7 +9887,7 @@
         <v>0.16381100000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="17" t="s">
         <v>151</v>
       </c>
@@ -9982,7 +9994,7 @@
         <v>7.2820000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="17" t="s">
         <v>153</v>
       </c>
@@ -10089,7 +10101,7 @@
         <v>4.7758000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>155</v>
       </c>
@@ -10196,7 +10208,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>158</v>
       </c>
@@ -10303,12 +10315,12 @@
         <v>2.1288000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
         <v>161</v>
       </c>
@@ -10415,7 +10427,7 @@
         <v>-9.4450000000000003E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
         <v>163</v>
       </c>
@@ -10522,7 +10534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="17" t="s">
         <v>165</v>
       </c>
@@ -10629,7 +10641,7 @@
         <v>-2.5900000000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="17" t="s">
         <v>166</v>
       </c>
@@ -10736,7 +10748,7 @@
         <v>-4.9399999999999997E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="17" t="s">
         <v>167</v>
       </c>
@@ -10843,7 +10855,7 @@
         <v>-1.6899999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>168</v>
       </c>
@@ -10950,12 +10962,12 @@
         <v>-1.0089999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="17" t="s">
         <v>170</v>
       </c>
@@ -11062,7 +11074,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="17" t="s">
         <v>171</v>
       </c>
@@ -11169,7 +11181,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="17" t="s">
         <v>172</v>
       </c>
@@ -11276,7 +11288,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="17" t="s">
         <v>173</v>
       </c>
@@ -11383,7 +11395,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="17" t="s">
         <v>174</v>
       </c>
@@ -11490,7 +11502,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
         <v>176</v>
       </c>
@@ -11597,7 +11609,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="17" t="s">
         <v>177</v>
       </c>
@@ -11704,7 +11716,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="17" t="s">
         <v>178</v>
       </c>
@@ -11811,7 +11823,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="17" t="s">
         <v>179</v>
       </c>
@@ -11918,7 +11930,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="17" t="s">
         <v>180</v>
       </c>
@@ -12025,7 +12037,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>182</v>
       </c>
@@ -12132,12 +12144,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="17" t="s">
         <v>184</v>
       </c>
@@ -12244,7 +12256,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="17" t="s">
         <v>185</v>
       </c>
@@ -12351,7 +12363,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="17" t="s">
         <v>186</v>
       </c>
@@ -12458,7 +12470,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="17" t="s">
         <v>187</v>
       </c>
@@ -12565,7 +12577,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="17" t="s">
         <v>188</v>
       </c>
@@ -12672,7 +12684,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="17" t="s">
         <v>189</v>
       </c>
@@ -12779,7 +12791,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="17" t="s">
         <v>190</v>
       </c>
@@ -12886,7 +12898,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="17" t="s">
         <v>191</v>
       </c>
@@ -12993,7 +13005,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="17" t="s">
         <v>192</v>
       </c>
@@ -13100,7 +13112,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="17" t="s">
         <v>193</v>
       </c>
@@ -13207,7 +13219,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>194</v>
       </c>
@@ -13314,7 +13326,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>195</v>
       </c>
@@ -13421,12 +13433,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="20" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="17" t="s">
         <v>198</v>
       </c>
@@ -13533,7 +13545,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="17" t="s">
         <v>199</v>
       </c>
@@ -13640,7 +13652,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="17" t="s">
         <v>200</v>
       </c>
@@ -13747,7 +13759,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="17" t="s">
         <v>201</v>
       </c>
@@ -13854,7 +13866,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="17" t="s">
         <v>202</v>
       </c>
@@ -13961,7 +13973,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="17" t="s">
         <v>203</v>
       </c>
@@ -14068,7 +14080,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="17" t="s">
         <v>204</v>
       </c>
@@ -14175,7 +14187,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="17" t="s">
         <v>205</v>
       </c>
@@ -14282,7 +14294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="17" t="s">
         <v>206</v>
       </c>
@@ -14389,7 +14401,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
         <v>207</v>
       </c>
@@ -14496,7 +14508,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
         <v>208</v>
       </c>
@@ -14603,12 +14615,12 @@
         <v>2.0830999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="20" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="17" t="s">
         <v>211</v>
       </c>
@@ -14715,7 +14727,7 @@
         <v>-1.1379999999999999E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="17" t="s">
         <v>212</v>
       </c>
@@ -14822,7 +14834,7 @@
         <v>-3.0509999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="17" t="s">
         <v>214</v>
       </c>
@@ -14929,7 +14941,7 @@
         <v>1.7583000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="17" t="s">
         <v>216</v>
       </c>
@@ -15036,7 +15048,7 @@
         <v>-1.436E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="17" t="s">
         <v>218</v>
       </c>
@@ -15143,7 +15155,7 @@
         <v>4.8812000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="17" t="s">
         <v>219</v>
       </c>
@@ -15250,7 +15262,7 @@
         <v>4.542E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>221</v>
       </c>
@@ -15357,7 +15369,7 @@
         <v>3.8552000000000003E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
         <v>222</v>
       </c>
@@ -15464,8 +15476,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="43" t="s">
         <v>224</v>
       </c>
@@ -15503,122 +15515,122 @@
       <c r="AH87" s="43"/>
       <c r="AI87" s="43"/>
     </row>
-    <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="26" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" s="26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="26" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="26" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B93" s="26" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="26" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="95" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="26" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="26" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="26" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B100" s="26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="26" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B102" s="26" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="26" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="26" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="26" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="26" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="26" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="26" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="26" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="26" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="26" t="s">
         <v>251</v>
       </c>
@@ -15637,17 +15649,17 @@
   <dimension ref="A1:AH68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.265625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="12.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A1" s="31" t="s">
         <v>304</v>
       </c>
@@ -15685,7 +15697,7 @@
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="B2">
         <v>2020</v>
       </c>
@@ -15783,7 +15795,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>305</v>
       </c>
@@ -15916,7 +15928,7 @@
         <v>4329.414625999998</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="27" t="s">
         <v>306</v>
       </c>
@@ -16049,149 +16061,149 @@
         <v>1384.6121700000003</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>260</v>
       </c>
       <c r="B6">
-        <f>-(B4-B$3)</f>
+        <f t="shared" ref="B6:AF6" si="1">-(B4-B$3)</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f>-(C4-C$3)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>-(D4-D$3)</f>
+        <f t="shared" si="1"/>
         <v>5.5654289999999946</v>
       </c>
       <c r="E6">
-        <f>-(E4-E$3)</f>
+        <f t="shared" si="1"/>
         <v>18.500381000000004</v>
       </c>
       <c r="F6">
-        <f>-(F4-F$3)</f>
+        <f t="shared" si="1"/>
         <v>40.273743000000024</v>
       </c>
       <c r="G6">
-        <f>-(G4-G$3)</f>
+        <f t="shared" si="1"/>
         <v>100.64464199999999</v>
       </c>
       <c r="H6">
-        <f>-(H4-H$3)</f>
+        <f t="shared" si="1"/>
         <v>101.659633</v>
       </c>
       <c r="I6">
-        <f>-(I4-I$3)</f>
+        <f t="shared" si="1"/>
         <v>103.75165899999999</v>
       </c>
       <c r="J6">
-        <f>-(J4-J$3)</f>
+        <f t="shared" si="1"/>
         <v>107.54541</v>
       </c>
       <c r="K6">
-        <f>-(K4-K$3)</f>
+        <f t="shared" si="1"/>
         <v>109.461716</v>
       </c>
       <c r="L6">
-        <f>-(L4-L$3)</f>
+        <f t="shared" si="1"/>
         <v>110.32470499999999</v>
       </c>
       <c r="M6">
-        <f>-(M4-M$3)</f>
+        <f t="shared" si="1"/>
         <v>110.32470999999998</v>
       </c>
       <c r="N6">
-        <f>-(N4-N$3)</f>
+        <f t="shared" si="1"/>
         <v>110.23240999999999</v>
       </c>
       <c r="O6">
-        <f>-(O4-O$3)</f>
+        <f t="shared" si="1"/>
         <v>111.022808</v>
       </c>
       <c r="P6">
-        <f>-(P4-P$3)</f>
+        <f t="shared" si="1"/>
         <v>112.61531400000001</v>
       </c>
       <c r="Q6">
-        <f>-(Q4-Q$3)</f>
+        <f t="shared" si="1"/>
         <v>112.615302</v>
       </c>
       <c r="R6">
-        <f>-(R4-R$3)</f>
+        <f t="shared" si="1"/>
         <v>111.932806</v>
       </c>
       <c r="S6">
-        <f>-(S4-S$3)</f>
+        <f t="shared" si="1"/>
         <v>111.737297</v>
       </c>
       <c r="T6">
-        <f>-(T4-T$3)</f>
+        <f t="shared" si="1"/>
         <v>111.819811</v>
       </c>
       <c r="U6">
-        <f>-(U4-U$3)</f>
+        <f t="shared" si="1"/>
         <v>112.264805</v>
       </c>
       <c r="V6">
-        <f>-(V4-V$3)</f>
+        <f t="shared" si="1"/>
         <v>112.264805</v>
       </c>
       <c r="W6">
-        <f>-(W4-W$3)</f>
+        <f t="shared" si="1"/>
         <v>113.41131</v>
       </c>
       <c r="X6">
-        <f>-(X4-X$3)</f>
+        <f t="shared" si="1"/>
         <v>113.41131</v>
       </c>
       <c r="Y6">
-        <f>-(Y4-Y$3)</f>
+        <f t="shared" si="1"/>
         <v>113.41131</v>
       </c>
       <c r="Z6">
-        <f>-(Z4-Z$3)</f>
+        <f t="shared" si="1"/>
         <v>113.41131</v>
       </c>
       <c r="AA6">
-        <f>-(AA4-AA$3)</f>
+        <f t="shared" si="1"/>
         <v>112.996301</v>
       </c>
       <c r="AB6">
-        <f>-(AB4-AB$3)</f>
+        <f t="shared" si="1"/>
         <v>112.996301</v>
       </c>
       <c r="AC6">
-        <f>-(AC4-AC$3)</f>
+        <f t="shared" si="1"/>
         <v>112.764306</v>
       </c>
       <c r="AD6">
-        <f>-(AD4-AD$3)</f>
+        <f t="shared" si="1"/>
         <v>112.764306</v>
       </c>
       <c r="AE6">
-        <f>-(AE4-AE$3)</f>
+        <f t="shared" si="1"/>
         <v>112.53930800000001</v>
       </c>
       <c r="AF6">
-        <f>-(AF4-AF$3)</f>
+        <f t="shared" si="1"/>
         <v>112.53930800000001</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="31" t="s">
         <v>282</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:34" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="57" x14ac:dyDescent="0.45">
       <c r="B9" s="27" t="s">
         <v>307</v>
       </c>
       <c r="C9" s="27"/>
     </row>
-    <row r="10" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="27" t="s">
         <v>261</v>
       </c>
@@ -16200,7 +16212,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="32" t="s">
         <v>285</v>
       </c>
@@ -16235,7 +16247,7 @@
       <c r="AD12" s="12"/>
       <c r="AE12" s="12"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>2021</v>
       </c>
@@ -16327,7 +16339,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="27" t="s">
         <v>280</v>
       </c>
@@ -16339,119 +16351,119 @@
         <v>36.75</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:AE14" si="1">C14*1.05</f>
+        <f t="shared" ref="D14:AE14" si="2">C14*1.05</f>
         <v>38.587499999999999</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.516874999999999</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42.542718749999999</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44.669854687499999</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46.903347421875004</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49.248514792968756</v>
       </c>
       <c r="J14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51.710940532617194</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54.296487559248057</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57.011311937210465</v>
       </c>
       <c r="M14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59.861877534070992</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62.854971410774546</v>
       </c>
       <c r="O14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65.997719981313281</v>
       </c>
       <c r="P14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69.297605980378947</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72.762486279397891</v>
       </c>
       <c r="R14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76.400610593367787</v>
       </c>
       <c r="S14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80.220641123036174</v>
       </c>
       <c r="T14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84.231673179187993</v>
       </c>
       <c r="U14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88.443256838147391</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.865419680054771</v>
       </c>
       <c r="W14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97.508690664057511</v>
       </c>
       <c r="X14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102.38412519726039</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107.50333145712341</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112.87849802997958</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.52242293147857</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.44854407805251</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130.67097128195513</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>137.2045198460529</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144.06474583835555</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>281</v>
       </c>
@@ -16460,123 +16472,123 @@
         <v>0.24294632108865083</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:AE15" si="2">C14/$AE14</f>
+        <f t="shared" ref="C15:AE15" si="3">C14/$AE14</f>
         <v>0.25509363714308336</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.26784831900023753</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28124073495024943</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.29530277169776187</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.31006791028264996</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.32557130579678251</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.34184987108662163</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.35894236464095275</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.37688948287300039</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.39573395701665043</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.41552065486748296</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.43629668761085716</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.45811152199140009</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.4810170980909701</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50506795299551854</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.53032135064529451</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.55683741817755927</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.58467928908643729</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.6139132535407591</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.64460891621779715</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.676839362028687</v>
       </c>
       <c r="X15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.71068133013012136</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74621539663662739</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.78352616646845885</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.82270247479188185</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.86383759853147601</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.90702947845804982</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.95238095238095233</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="33" t="s">
         <v>279</v>
       </c>
@@ -16584,154 +16596,173 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B21">
+        <v>3452.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B22">
+        <v>233797.7999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" s="1">
+        <f>B21/B22</f>
+        <v>1.4766606015967651E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68"/>
     </row>
   </sheetData>
@@ -16743,21 +16774,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ119"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="68.59765625" customWidth="1"/>
+    <col min="2" max="2" width="39.73046875" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="36" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A1" s="11" t="s">
         <v>121</v>
       </c>
@@ -16797,7 +16828,7 @@
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -16815,7 +16846,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="35" t="s">
         <v>41</v>
       </c>
@@ -16865,7 +16896,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -16925,7 +16956,7 @@
         <v>44089.664454448415</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -16985,7 +17016,7 @@
         <v>43540.396738428462</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -17045,7 +17076,7 @@
         <v>42632.18015665796</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -17105,7 +17136,7 @@
         <v>41615.725567188492</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -17165,7 +17196,7 @@
         <v>40875.078718752076</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -17203,7 +17234,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -17241,7 +17272,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -17279,7 +17310,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -17317,7 +17348,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -17355,7 +17386,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -17393,7 +17424,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -17431,7 +17462,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -17469,7 +17500,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -17507,7 +17538,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -17545,22 +17576,22 @@
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>2019</v>
       </c>
@@ -17658,7 +17689,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -17759,7 +17790,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>71</v>
       </c>
@@ -17860,7 +17891,7 @@
         <v>1.80877E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>72</v>
       </c>
@@ -17961,7 +17992,7 @@
         <v>4.0960000000000003E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>73</v>
       </c>
@@ -18062,7 +18093,7 @@
         <v>6.5560000000000002E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>74</v>
       </c>
@@ -18163,7 +18194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>75</v>
       </c>
@@ -18264,7 +18295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>76</v>
       </c>
@@ -18365,7 +18396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>77</v>
       </c>
@@ -18466,7 +18497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>78</v>
       </c>
@@ -18567,7 +18598,7 @@
         <v>2.03E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>79</v>
       </c>
@@ -18668,7 +18699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>80</v>
       </c>
@@ -18769,7 +18800,7 @@
         <v>2.1129999999999999E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>81</v>
       </c>
@@ -18870,7 +18901,7 @@
         <v>4.0960000000000003E-6</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>82</v>
       </c>
@@ -18971,7 +19002,7 @@
         <v>1.6589999999999999E-6</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>83</v>
       </c>
@@ -19072,7 +19103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>84</v>
       </c>
@@ -19173,7 +19204,7 @@
         <v>1.5820000000000001E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>85</v>
       </c>
@@ -19274,7 +19305,7 @@
         <v>1.6140000000000001E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>86</v>
       </c>
@@ -19375,12 +19406,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>2019</v>
       </c>
@@ -19478,7 +19509,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -19579,7 +19610,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>87</v>
       </c>
@@ -19680,7 +19711,7 @@
         <v>10375000</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>88</v>
       </c>
@@ -19781,7 +19812,7 @@
         <v>6516500</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>89</v>
       </c>
@@ -19882,7 +19913,7 @@
         <v>10450000</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -19983,7 +20014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -20084,7 +20115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>92</v>
       </c>
@@ -20185,7 +20216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -20286,7 +20317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>94</v>
       </c>
@@ -20387,7 +20418,7 @@
         <v>14500000</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>95</v>
       </c>
@@ -20488,7 +20519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>96</v>
       </c>
@@ -20589,7 +20620,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>97</v>
       </c>
@@ -20690,7 +20721,7 @@
         <v>8902000</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>98</v>
       </c>
@@ -20791,7 +20822,7 @@
         <v>10928800</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>99</v>
       </c>
@@ -20892,7 +20923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>100</v>
       </c>
@@ -20993,7 +21024,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A62" s="9" t="s">
         <v>101</v>
       </c>
@@ -21094,7 +21125,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>102</v>
       </c>
@@ -21195,12 +21226,12 @@
         <v>14500000</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>40</v>
       </c>
@@ -21301,7 +21332,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -21402,7 +21433,7 @@
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -21503,7 +21534,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>105</v>
       </c>
@@ -21604,7 +21635,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -21705,7 +21736,7 @@
         <v>0.46100000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>107</v>
       </c>
@@ -21806,7 +21837,7 @@
         <v>0.33476600000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>108</v>
       </c>
@@ -21907,7 +21938,7 @@
         <v>0.217416</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>109</v>
       </c>
@@ -22008,7 +22039,7 @@
         <v>0.61199999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>110</v>
       </c>
@@ -22109,7 +22140,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>111</v>
       </c>
@@ -22210,7 +22241,7 @@
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>112</v>
       </c>
@@ -22311,7 +22342,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>113</v>
       </c>
@@ -22412,7 +22443,7 @@
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>114</v>
       </c>
@@ -22513,7 +22544,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>115</v>
       </c>
@@ -22614,7 +22645,7 @@
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>116</v>
       </c>
@@ -22715,7 +22746,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>117</v>
       </c>
@@ -22816,7 +22847,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>118</v>
       </c>
@@ -22917,12 +22948,12 @@
         <v>1.002</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -22931,7 +22962,7 @@
         <v>37.91957141830045</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -22940,7 +22971,7 @@
         <v>22.066844467696896</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -22949,7 +22980,7 @@
         <v>23.690599400839194</v>
       </c>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>25</v>
       </c>
@@ -22958,7 +22989,7 @@
         <v>11.698640141047356</v>
       </c>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -22967,7 +22998,7 @@
         <v>8.196236123322107</v>
       </c>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>119</v>
       </c>
@@ -22976,7 +23007,7 @@
         <v>7.6743450535082207</v>
       </c>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>120</v>
       </c>
@@ -22985,7 +23016,7 @@
         <v>15.860491837526487</v>
       </c>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>29</v>
       </c>
@@ -22994,7 +23025,7 @@
         <v>55.261317485898473</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>30</v>
       </c>
@@ -23003,7 +23034,7 @@
         <v>16.629675121802013</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>31</v>
       </c>
@@ -23012,7 +23043,7 @@
         <v>213.61222031963467</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>32</v>
       </c>
@@ -23021,7 +23052,7 @@
         <v>36.38234998570578</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>62</v>
       </c>
@@ -23030,7 +23061,7 @@
         <v>40.844083378801315</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>64</v>
       </c>
@@ -23039,7 +23070,7 @@
         <v>26.548972845107564</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>66</v>
       </c>
@@ -23048,7 +23079,7 @@
         <v>105.26222031963468</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>67</v>
       </c>
@@ -23057,7 +23088,7 @@
         <v>128.31222031963472</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>68</v>
       </c>
@@ -23066,12 +23097,12 @@
         <v>8.4508264749040727</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -23080,7 +23111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>23</v>
       </c>
@@ -23089,7 +23120,7 @@
         <v>0.58193812963421754</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -23098,7 +23129,7 @@
         <v>0.62475915509440116</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>25</v>
       </c>
@@ -23107,7 +23138,7 @@
         <v>0.30851192942021094</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>26</v>
       </c>
@@ -23116,7 +23147,7 @@
         <v>0.21614791034706957</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>119</v>
       </c>
@@ -23125,7 +23156,7 @@
         <v>0.20238480463955053</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>120</v>
       </c>
@@ -23134,7 +23165,7 @@
         <v>0.41826664290493587</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>29</v>
       </c>
@@ -23143,7 +23174,7 @@
         <v>1.4573296959582376</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>30</v>
       </c>
@@ -23152,7 +23183,7 @@
         <v>0.43855124147780655</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>31</v>
       </c>
@@ -23161,7 +23192,7 @@
         <v>5.6332973272093154</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>32</v>
       </c>
@@ -23170,7 +23201,7 @@
         <v>0.95946100192860329</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>62</v>
       </c>
@@ -23179,7 +23210,7 @@
         <v>1.0771240773857866</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>64</v>
       </c>
@@ -23188,7 +23219,7 @@
         <v>0.70013905358367801</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>66</v>
       </c>
@@ -23197,7 +23228,7 @@
         <v>2.775933808915199</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>67</v>
       </c>
@@ -23206,7 +23237,7 @@
         <v>3.3837993289583879</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>68</v>
       </c>
@@ -23231,102 +23262,102 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="5">
-        <f>Calculations!$B$17*Weighting!B104</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B104*Calculations!$B$23</f>
+        <v>59.066424063870599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="5">
-        <f>Calculations!$B$17*Weighting!B105</f>
-        <v>2327.75251853687</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B105*Calculations!$B$23</f>
+        <v>34.373004343910395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="5">
-        <f>Calculations!$B$17*Weighting!B106</f>
-        <v>2499.0366203776048</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B106*Calculations!$B$23</f>
+        <v>36.902289192591404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="5">
-        <f>Calculations!$B$17*Weighting!B107</f>
-        <v>1234.0477176808438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B107*Calculations!$B$23</f>
+        <v>18.222696451897097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="5">
-        <f>Calculations!$B$17*Weighting!B108</f>
-        <v>864.59164138827828</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B108*Calculations!$B$23</f>
+        <v>12.767084133079496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="5">
-        <f>Calculations!$B$17*Weighting!B109</f>
-        <v>809.53921855820215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B109*Calculations!$B$23</f>
+        <v>11.954146694923299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="5">
-        <f>Calculations!$B$17*Weighting!B110</f>
-        <v>1673.0665716197434</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B110*Calculations!$B$23</f>
+        <v>24.705514901594476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="5">
-        <f>Calculations!$B$17*Weighting!B111</f>
-        <v>5829.3187838329504</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B111*Calculations!$B$23</f>
+        <v>86.079253822340874</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="5">
-        <f>Calculations!$B$17*Weighting!B112</f>
-        <v>1754.2049659112263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B112*Calculations!$B$23</f>
+        <v>25.903653602865042</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
@@ -23334,7 +23365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
@@ -23342,25 +23373,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="5">
-        <f>Calculations!$B$17*Weighting!B115</f>
-        <v>4308.4963095431467</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B115*Calculations!$B$23</f>
+        <v>63.621867524274251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="5">
-        <f>Calculations!$B$17*Weighting!B116</f>
-        <v>2800.556214334712</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <f>Calculations!$B$17*Weighting!B116*Calculations!$B$23</f>
+        <v>41.354710242650548</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -23368,7 +23399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -23376,13 +23407,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="5">
-        <f>Calculations!$B$17*Weighting!B119</f>
-        <v>891.44746723857747</v>
+        <f>Calculations!$B$17*Weighting!B119*Calculations!$B$23</f>
+        <v>13.163653532644304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>